<commit_message>
Functioning heat and elec demand
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mreuter/Documents/GitHub/ESEM----EE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314D2727-F6B9-5249-BD52-FD245A916E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51FD018-9A24-3E45-A3BA-62248A968357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16120" activeTab="1" xr2:uid="{AA20818D-C879-3C47-BB4F-616D309467DF}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16120" activeTab="4" xr2:uid="{AA20818D-C879-3C47-BB4F-616D309467DF}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
     <sheet name="provinces" sheetId="2" r:id="rId2"/>
+    <sheet name="elec_slp" sheetId="3" r:id="rId3"/>
+    <sheet name="heat_slp" sheetId="4" r:id="rId4"/>
+    <sheet name="heat_prov" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="91">
   <si>
     <t>id</t>
   </si>
@@ -138,13 +141,184 @@
   </si>
   <si>
     <t>Thüringen</t>
+  </si>
+  <si>
+    <t>sector_id</t>
+  </si>
+  <si>
+    <t>sector</t>
+  </si>
+  <si>
+    <t>g0</t>
+  </si>
+  <si>
+    <t>Gewerbe allg.</t>
+  </si>
+  <si>
+    <t>g1</t>
+  </si>
+  <si>
+    <t>Gewerbe werktags</t>
+  </si>
+  <si>
+    <t>g2</t>
+  </si>
+  <si>
+    <t>Gewerbe Abendstd.</t>
+  </si>
+  <si>
+    <t>g3</t>
+  </si>
+  <si>
+    <t>Gewerbe durchlaufend</t>
+  </si>
+  <si>
+    <t>g4</t>
+  </si>
+  <si>
+    <t>Laden/Friseur</t>
+  </si>
+  <si>
+    <t>g5</t>
+  </si>
+  <si>
+    <t>Bäckerei</t>
+  </si>
+  <si>
+    <t>g6</t>
+  </si>
+  <si>
+    <t>Wochenendbetrieb</t>
+  </si>
+  <si>
+    <t>h0</t>
+  </si>
+  <si>
+    <t>Haushalt</t>
+  </si>
+  <si>
+    <t>l0</t>
+  </si>
+  <si>
+    <t>Landwirtschaftsbetriebe</t>
+  </si>
+  <si>
+    <t>l1</t>
+  </si>
+  <si>
+    <t>Landwirt. + Milchwirt./Tierzucht</t>
+  </si>
+  <si>
+    <t>l2</t>
+  </si>
+  <si>
+    <t>Landwirtschaft sonst.</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>EFH</t>
+  </si>
+  <si>
+    <t>Einfamilienhaus</t>
+  </si>
+  <si>
+    <t>MFH</t>
+  </si>
+  <si>
+    <t>Mehrfamilienhaus</t>
+  </si>
+  <si>
+    <t>GMK</t>
+  </si>
+  <si>
+    <t>Metall und Kfz</t>
+  </si>
+  <si>
+    <t>GHA</t>
+  </si>
+  <si>
+    <t>Einzel- und Großhandel</t>
+  </si>
+  <si>
+    <t>GKO</t>
+  </si>
+  <si>
+    <t>Gebietskörperschaften</t>
+  </si>
+  <si>
+    <t>GBD</t>
+  </si>
+  <si>
+    <t>sonstige betriebliche Diensleistung</t>
+  </si>
+  <si>
+    <t>GGA</t>
+  </si>
+  <si>
+    <t>Gaststätten</t>
+  </si>
+  <si>
+    <t>GBH</t>
+  </si>
+  <si>
+    <t>Beherbergung</t>
+  </si>
+  <si>
+    <t>GWA</t>
+  </si>
+  <si>
+    <t>Wäschereien</t>
+  </si>
+  <si>
+    <t>GGB</t>
+  </si>
+  <si>
+    <t>Gartenbau</t>
+  </si>
+  <si>
+    <t>GBA</t>
+  </si>
+  <si>
+    <t>Backstube</t>
+  </si>
+  <si>
+    <t>GPD</t>
+  </si>
+  <si>
+    <t>Papier und Druck</t>
+  </si>
+  <si>
+    <t>GMF</t>
+  </si>
+  <si>
+    <t>haushaltsähnliche Gewerbebetriebe</t>
+  </si>
+  <si>
+    <t>GHD</t>
+  </si>
+  <si>
+    <t>Summenlastprofil Gewerbe/Handel/Dienstleistungn</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>windy</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>Deutschland</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -160,8 +334,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,8 +377,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBDD7EE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5B9BD5"/>
+        <bgColor rgb="FF5B9BD5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor rgb="FFDDEBF7"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -189,15 +404,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF9BC2E6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF9BC2E6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF9BC2E6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF9BC2E6"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -213,6 +452,105 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>778701</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>144101</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6607175" y="494594"/>
+          <a:ext cx="5553901" cy="3496901"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>143707</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>35736</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7569199" y="4390675"/>
+          <a:ext cx="4830007" cy="2677336"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -533,7 +871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{005AEBD3-4FB1-9142-9700-8095D138010F}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
@@ -683,4 +1021,1035 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C565C1AA-04DB-BA45-B55A-2F87B5B6FC2B}">
+  <dimension ref="A1:L13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.83203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F4FC067-D7E2-4E47-B0D2-E6A837753E63}">
+  <dimension ref="B2:C16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="9.1640625" style="2"/>
+    <col min="3" max="3" width="48.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.1640625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F568D1CF-900F-154E-8444-949F6BB9AE2C}">
+  <dimension ref="A1:N38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="6"/>
+      <c r="B3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="5">
+        <v>4</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="6"/>
+      <c r="B4" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="5">
+        <v>5</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="6"/>
+      <c r="B5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="5">
+        <v>3</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="6"/>
+      <c r="B6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="5">
+        <v>5</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="6"/>
+      <c r="B7" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="6"/>
+      <c r="B8" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="5">
+        <v>11</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="6"/>
+      <c r="B9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="5">
+        <v>2</v>
+      </c>
+      <c r="E9" s="5">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="6"/>
+      <c r="B10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="5">
+        <v>3</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="6"/>
+      <c r="B11" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="5">
+        <v>6</v>
+      </c>
+      <c r="E11" s="5">
+        <v>1</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="6"/>
+      <c r="B12" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="5">
+        <v>3</v>
+      </c>
+      <c r="E12" s="5">
+        <v>1</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="6"/>
+      <c r="B13" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="5">
+        <v>3</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="6"/>
+      <c r="B14" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="5">
+        <v>4</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="6"/>
+      <c r="B15" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="5">
+        <v>2</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="6"/>
+      <c r="B16" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="5">
+        <v>4</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="6"/>
+      <c r="B17" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="5">
+        <v>5</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0</v>
+      </c>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="6"/>
+      <c r="B18" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="5">
+        <v>4</v>
+      </c>
+      <c r="E18" s="5">
+        <v>1</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="6"/>
+      <c r="B19" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="5">
+        <v>5</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0</v>
+      </c>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="6"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="6"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="6"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="6"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="6"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="6"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="6"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="6"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="6"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="6"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" s="6"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" s="6"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" s="6"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" s="6"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" s="6"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" s="6"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" s="6"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" s="6"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="5"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" s="6"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Functioning PV (scaled by area)
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mreuter/Documents/GitHub/ESEM----EE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51FD018-9A24-3E45-A3BA-62248A968357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E14F702-25AD-6543-81E9-8FC93965D2AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16120" activeTab="4" xr2:uid="{AA20818D-C879-3C47-BB4F-616D309467DF}"/>
+    <workbookView xWindow="1120" yWindow="500" windowWidth="28040" windowHeight="16120" activeTab="1" xr2:uid="{AA20818D-C879-3C47-BB4F-616D309467DF}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
-    <sheet name="provinces" sheetId="2" r:id="rId2"/>
-    <sheet name="elec_slp" sheetId="3" r:id="rId3"/>
-    <sheet name="heat_slp" sheetId="4" r:id="rId4"/>
-    <sheet name="heat_prov" sheetId="5" r:id="rId5"/>
+    <sheet name="tech" sheetId="7" r:id="rId2"/>
+    <sheet name="provinces" sheetId="2" r:id="rId3"/>
+    <sheet name="elec_slp" sheetId="3" r:id="rId4"/>
+    <sheet name="heat_slp" sheetId="4" r:id="rId5"/>
+    <sheet name="heat_prov" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="115">
   <si>
     <t>id</t>
   </si>
@@ -312,13 +313,85 @@
   </si>
   <si>
     <t>Deutschland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id </t>
+  </si>
+  <si>
+    <t>ef</t>
+  </si>
+  <si>
+    <t>G_100</t>
+  </si>
+  <si>
+    <t>G_50</t>
+  </si>
+  <si>
+    <t>G_DE</t>
+  </si>
+  <si>
+    <t>PV</t>
+  </si>
+  <si>
+    <t>Wind</t>
+  </si>
+  <si>
+    <t>CHB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaskessel </t>
+  </si>
+  <si>
+    <t>HP_Air</t>
+  </si>
+  <si>
+    <t>HP_Water</t>
+  </si>
+  <si>
+    <t>HP_Ground</t>
+  </si>
+  <si>
+    <t>FW</t>
+  </si>
+  <si>
+    <t>Fernwärme</t>
+  </si>
+  <si>
+    <t>Wärmepumpe Luft</t>
+  </si>
+  <si>
+    <t>Wärmepumpe Grundwasser</t>
+  </si>
+  <si>
+    <t>Wärmepumpe Sole</t>
+  </si>
+  <si>
+    <t>Klein-Windkraftanlage</t>
+  </si>
+  <si>
+    <t>Photovoltaic Module</t>
+  </si>
+  <si>
+    <t>Deutschland-Mix Netzstrom</t>
+  </si>
+  <si>
+    <t>Netzstrom 50% Ökostrom</t>
+  </si>
+  <si>
+    <t>Netzstrom 100% Ökostrom</t>
+  </si>
+  <si>
+    <t>(price)</t>
+  </si>
+  <si>
+    <t>info</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -353,6 +426,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -423,7 +504,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -437,6 +518,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -868,6 +950,123 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CAE16E0-8D9A-B945-AFD0-7E1B2FCCBD6C}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="24.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{005AEBD3-4FB1-9142-9700-8095D138010F}">
   <dimension ref="A1:C18"/>
   <sheetViews>
@@ -1023,7 +1222,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C565C1AA-04DB-BA45-B55A-2F87B5B6FC2B}">
   <dimension ref="A1:L13"/>
   <sheetViews>
@@ -1146,7 +1345,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F4FC067-D7E2-4E47-B0D2-E6A837753E63}">
   <dimension ref="B2:C16"/>
   <sheetViews>
@@ -1286,11 +1485,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F568D1CF-900F-154E-8444-949F6BB9AE2C}">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Functioning co2 comp calc
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mreuter/Documents/GitHub/ESEM----EE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E14F702-25AD-6543-81E9-8FC93965D2AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5063A75E-E0A2-7441-8C23-5E147D5B40B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="500" windowWidth="28040" windowHeight="16120" activeTab="1" xr2:uid="{AA20818D-C879-3C47-BB4F-616D309467DF}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16120" activeTab="1" xr2:uid="{AA20818D-C879-3C47-BB4F-616D309467DF}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
     <sheet name="tech" sheetId="7" r:id="rId2"/>
-    <sheet name="provinces" sheetId="2" r:id="rId3"/>
-    <sheet name="elec_slp" sheetId="3" r:id="rId4"/>
-    <sheet name="heat_slp" sheetId="4" r:id="rId5"/>
-    <sheet name="heat_prov" sheetId="5" r:id="rId6"/>
+    <sheet name="soltherm_data" sheetId="8" r:id="rId3"/>
+    <sheet name="provinces" sheetId="2" r:id="rId4"/>
+    <sheet name="elec_slp" sheetId="3" r:id="rId5"/>
+    <sheet name="heat_slp" sheetId="4" r:id="rId6"/>
+    <sheet name="heat_prov" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="130">
   <si>
     <t>id</t>
   </si>
@@ -324,9 +325,6 @@
     <t>G_100</t>
   </si>
   <si>
-    <t>G_50</t>
-  </si>
-  <si>
     <t>G_DE</t>
   </si>
   <si>
@@ -375,23 +373,71 @@
     <t>Deutschland-Mix Netzstrom</t>
   </si>
   <si>
-    <t>Netzstrom 50% Ökostrom</t>
-  </si>
-  <si>
     <t>Netzstrom 100% Ökostrom</t>
   </si>
   <si>
-    <t>(price)</t>
-  </si>
-  <si>
     <t>info</t>
+  </si>
+  <si>
+    <t>quality</t>
+  </si>
+  <si>
+    <t>collector_type</t>
+  </si>
+  <si>
+    <t>collector_tilt</t>
+  </si>
+  <si>
+    <t>collector_azimuth</t>
+  </si>
+  <si>
+    <t>eta_0</t>
+  </si>
+  <si>
+    <t>a_1</t>
+  </si>
+  <si>
+    <t>a_2</t>
+  </si>
+  <si>
+    <t>temp_collector_inlet</t>
+  </si>
+  <si>
+    <t>delta_temp_n</t>
+  </si>
+  <si>
+    <t>flat_low</t>
+  </si>
+  <si>
+    <t>flat_high</t>
+  </si>
+  <si>
+    <t>tube</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flat </t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>is the average of flat_high and flat_low!</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>tarif</t>
+  </si>
+  <si>
+    <t>lcoe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -438,8 +484,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -476,6 +529,12 @@
         <bgColor rgb="FFDDEBF7"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -504,7 +563,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -519,6 +578,10 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -951,10 +1014,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CAE16E0-8D9A-B945-AFD0-7E1B2FCCBD6C}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -963,8 +1026,8 @@
     <col min="3" max="3" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" s="11" t="s">
         <v>91</v>
       </c>
@@ -975,90 +1038,145 @@
         <v>92</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>93</v>
       </c>
       <c r="C3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+      <c r="D3">
+        <v>30</v>
+      </c>
+      <c r="F3">
+        <v>32.54</v>
+      </c>
+      <c r="G3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>94</v>
       </c>
       <c r="C4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+      <c r="D4">
+        <v>400</v>
+      </c>
+      <c r="F4">
+        <v>32.630000000000003</v>
+      </c>
+      <c r="G4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>95</v>
       </c>
       <c r="C5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+      <c r="D5">
+        <v>50</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>96</v>
       </c>
       <c r="C6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>97</v>
       </c>
       <c r="C7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="D7">
+        <v>247</v>
+      </c>
+      <c r="F7">
+        <v>9.5</v>
+      </c>
+      <c r="G7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+      <c r="E8">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>100</v>
       </c>
       <c r="C9" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>101</v>
       </c>
       <c r="C10" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>102</v>
       </c>
       <c r="C11" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
         <v>103</v>
       </c>
-      <c r="C12" t="s">
-        <v>104</v>
+      <c r="D11">
+        <v>198</v>
+      </c>
+      <c r="F11">
+        <v>9.1999999999999993</v>
       </c>
     </row>
   </sheetData>
@@ -1067,6 +1185,190 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9E424A2-3675-FF47-8266-60B248167A50}">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="13"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="13"/>
+      <c r="B2" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="13"/>
+      <c r="B3" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="12">
+        <v>45</v>
+      </c>
+      <c r="D3" s="12">
+        <v>20</v>
+      </c>
+      <c r="E3" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="F3" s="12">
+        <v>3.24</v>
+      </c>
+      <c r="G3" s="12">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H3" s="13">
+        <v>20</v>
+      </c>
+      <c r="I3" s="13">
+        <v>10</v>
+      </c>
+      <c r="J3" s="12"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="13"/>
+      <c r="B4" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="12">
+        <v>45</v>
+      </c>
+      <c r="D4" s="12">
+        <v>20</v>
+      </c>
+      <c r="E4" s="12">
+        <v>0.74</v>
+      </c>
+      <c r="F4" s="12">
+        <v>2.37</v>
+      </c>
+      <c r="G4" s="12">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H4" s="13">
+        <v>20</v>
+      </c>
+      <c r="I4" s="13">
+        <v>10</v>
+      </c>
+      <c r="J4" s="12"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="13"/>
+      <c r="B5" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="12">
+        <v>45</v>
+      </c>
+      <c r="D5" s="12">
+        <v>20</v>
+      </c>
+      <c r="E5" s="12">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="F5" s="12">
+        <v>0.62</v>
+      </c>
+      <c r="G5" s="12">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H5" s="13">
+        <v>20</v>
+      </c>
+      <c r="I5" s="13">
+        <v>10</v>
+      </c>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="12">
+        <v>45</v>
+      </c>
+      <c r="D6" s="12">
+        <v>20</v>
+      </c>
+      <c r="E6" s="12">
+        <f>AVERAGE(E3:E4)</f>
+        <v>0.77</v>
+      </c>
+      <c r="F6" s="12">
+        <f>AVERAGE(F3:F4)</f>
+        <v>2.8050000000000002</v>
+      </c>
+      <c r="G6" s="12">
+        <f>AVERAGE(G3:G4)</f>
+        <v>0.01</v>
+      </c>
+      <c r="H6" s="13">
+        <v>20</v>
+      </c>
+      <c r="I6" s="13">
+        <v>10</v>
+      </c>
+      <c r="J6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="E6:G6" formulaRange="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{005AEBD3-4FB1-9142-9700-8095D138010F}">
   <dimension ref="A1:C18"/>
   <sheetViews>
@@ -1222,7 +1524,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C565C1AA-04DB-BA45-B55A-2F87B5B6FC2B}">
   <dimension ref="A1:L13"/>
   <sheetViews>
@@ -1345,7 +1647,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F4FC067-D7E2-4E47-B0D2-E6A837753E63}">
   <dimension ref="B2:C16"/>
   <sheetViews>
@@ -1485,7 +1787,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F568D1CF-900F-154E-8444-949F6BB9AE2C}">
   <dimension ref="A1:N38"/>
   <sheetViews>

</xml_diff>

<commit_message>
ERA5 API - Implementation (Buggy)
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0e24e2a113d23d62/Dokumente/GitHub/ESEM-EE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mreuter/Documents/GitHub/ESEM----EE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{5063A75E-E0A2-7441-8C23-5E147D5B40B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E14B5A33-DB0C-46E3-AF0A-EC2DD2DB15E3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6919FBE6-99CC-3541-96DE-05FA34DA3742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="9030" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{AA20818D-C879-3C47-BB4F-616D309467DF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" activeTab="3" xr2:uid="{AA20818D-C879-3C47-BB4F-616D309467DF}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
     <sheet name="tech" sheetId="7" r:id="rId2"/>
     <sheet name="soltherm_data" sheetId="8" r:id="rId3"/>
-    <sheet name="provinces" sheetId="2" r:id="rId4"/>
-    <sheet name="elec_slp" sheetId="3" r:id="rId5"/>
-    <sheet name="co2" sheetId="9" r:id="rId6"/>
-    <sheet name="heat_slp" sheetId="4" r:id="rId7"/>
-    <sheet name="heat_prov" sheetId="5" r:id="rId8"/>
+    <sheet name="wind" sheetId="10" r:id="rId4"/>
+    <sheet name="provinces" sheetId="2" r:id="rId5"/>
+    <sheet name="elec_slp" sheetId="3" r:id="rId6"/>
+    <sheet name="co2" sheetId="9" r:id="rId7"/>
+    <sheet name="heat_slp" sheetId="4" r:id="rId8"/>
+    <sheet name="heat_prov" sheetId="5" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="139">
   <si>
     <t>id</t>
   </si>
@@ -450,6 +451,15 @@
   </si>
   <si>
     <t>average of flat_high and flat_low</t>
+  </si>
+  <si>
+    <t>wind_speed</t>
+  </si>
+  <si>
+    <t>power</t>
+  </si>
+  <si>
+    <t>power_coefficient</t>
   </si>
 </sst>
 </file>
@@ -511,7 +521,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -584,6 +594,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -612,7 +628,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -640,6 +656,7 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1059,12 +1076,12 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1078,15 +1095,15 @@
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="11" style="1"/>
     <col min="3" max="3" width="24.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" s="10" t="s">
         <v>89</v>
       </c>
@@ -1109,7 +1126,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>91</v>
       </c>
@@ -1130,7 +1147,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>92</v>
       </c>
@@ -1151,7 +1168,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>93</v>
       </c>
@@ -1172,7 +1189,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>94</v>
       </c>
@@ -1193,7 +1210,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>95</v>
       </c>
@@ -1214,7 +1231,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>97</v>
       </c>
@@ -1231,7 +1248,7 @@
       </c>
       <c r="H8"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>98</v>
       </c>
@@ -1248,7 +1265,7 @@
       </c>
       <c r="H9"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>99</v>
       </c>
@@ -1265,7 +1282,7 @@
       </c>
       <c r="H10"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>100</v>
       </c>
@@ -1293,24 +1310,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9E424A2-3675-FF47-8266-60B248167A50}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.25" style="13" customWidth="1"/>
+    <col min="1" max="1" width="4.1640625" style="13" customWidth="1"/>
     <col min="2" max="2" width="12.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.375" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" style="13" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="11" style="13"/>
-    <col min="8" max="8" width="17.875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" style="13" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.25" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.1640625" style="13" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="12"/>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -1322,7 +1339,7 @@
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="12"/>
       <c r="B2" s="19" t="s">
         <v>111</v>
@@ -1352,7 +1369,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="12"/>
       <c r="B3" s="11" t="s">
         <v>119</v>
@@ -1380,7 +1397,7 @@
       </c>
       <c r="J3" s="11"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
       <c r="B4" s="11" t="s">
         <v>120</v>
@@ -1408,7 +1425,7 @@
       </c>
       <c r="J4" s="11"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
       <c r="B5" s="11" t="s">
         <v>121</v>
@@ -1436,7 +1453,7 @@
       </c>
       <c r="J5" s="11"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B6" s="11" t="s">
         <v>122</v>
       </c>
@@ -1478,6 +1495,298 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26567F63-836F-5244-9500-1ED5AA3A6D06}">
+  <dimension ref="A1:D23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="23"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" s="23" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <f>C3/20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <f>B4*2</f>
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <f>C4/30</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:C23" si="0">B5*2</f>
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:D10" si="1">C5/30</f>
+        <v>0.13333333333333333</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <f>C7/30</f>
+        <v>0.26666666666666666</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <f>C9/30</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>0.46666666666666667</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <f>C11/30</f>
+        <v>0.53333333333333333</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D12">
+        <f>0.55</f>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D13">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="D14">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D15">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="D16">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="D17">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D18">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="D19">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>17</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="D20">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>18</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="D21">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>19</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="D22">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D23">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{005AEBD3-4FB1-9142-9700-8095D138010F}">
   <dimension ref="B2:C18"/>
   <sheetViews>
@@ -1485,14 +1794,14 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9.125" style="2"/>
-    <col min="3" max="3" width="26.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.125" style="2"/>
+    <col min="1" max="2" width="9.1640625" style="2"/>
+    <col min="3" max="3" width="26.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1500,7 +1809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -1508,7 +1817,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -1516,7 +1825,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -1524,7 +1833,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>8</v>
       </c>
@@ -1532,7 +1841,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>10</v>
       </c>
@@ -1540,7 +1849,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -1548,7 +1857,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>14</v>
       </c>
@@ -1556,7 +1865,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>16</v>
       </c>
@@ -1564,7 +1873,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>18</v>
       </c>
@@ -1572,7 +1881,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>20</v>
       </c>
@@ -1580,7 +1889,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>22</v>
       </c>
@@ -1588,7 +1897,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>24</v>
       </c>
@@ -1596,7 +1905,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>26</v>
       </c>
@@ -1604,7 +1913,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>28</v>
       </c>
@@ -1612,7 +1921,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>30</v>
       </c>
@@ -1620,7 +1929,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>32</v>
       </c>
@@ -1633,7 +1942,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C565C1AA-04DB-BA45-B55A-2F87B5B6FC2B}">
   <dimension ref="B2:L13"/>
   <sheetViews>
@@ -1641,15 +1950,15 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="2"/>
-    <col min="3" max="3" width="29.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.125" style="2"/>
+    <col min="1" max="1" width="3.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="2"/>
+    <col min="3" max="3" width="29.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1664,7 +1973,7 @@
       <c r="K2" s="20"/>
       <c r="L2" s="20"/>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>34</v>
       </c>
@@ -1672,7 +1981,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>36</v>
       </c>
@@ -1680,7 +1989,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>38</v>
       </c>
@@ -1688,7 +1997,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>40</v>
       </c>
@@ -1696,7 +2005,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>42</v>
       </c>
@@ -1704,7 +2013,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>44</v>
       </c>
@@ -1712,7 +2021,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>46</v>
       </c>
@@ -1720,7 +2029,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>48</v>
       </c>
@@ -1728,7 +2037,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>50</v>
       </c>
@@ -1736,7 +2045,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>52</v>
       </c>
@@ -1744,7 +2053,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>54</v>
       </c>
@@ -1757,7 +2066,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DB8F52B-EB96-459B-BB6A-A07D4250C420}">
   <dimension ref="B2:L6"/>
   <sheetViews>
@@ -1765,15 +2074,15 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.875" style="21" customWidth="1"/>
+    <col min="1" max="1" width="3.83203125" style="21" customWidth="1"/>
     <col min="2" max="2" width="11" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.875" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.125" style="21"/>
+    <col min="3" max="3" width="29.83203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.1640625" style="21"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1788,7 +2097,7 @@
       <c r="K2" s="22"/>
       <c r="L2" s="22"/>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>127</v>
       </c>
@@ -1796,7 +2105,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4" s="14" t="s">
         <v>128</v>
       </c>
@@ -1804,7 +2113,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>129</v>
       </c>
@@ -1812,7 +2121,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>130</v>
       </c>
@@ -1825,7 +2134,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F4FC067-D7E2-4E47-B0D2-E6A837753E63}">
   <dimension ref="B2:C16"/>
   <sheetViews>
@@ -1833,14 +2142,14 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9.125" style="2"/>
-    <col min="3" max="3" width="48.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.125" style="2"/>
+    <col min="1" max="2" width="9.1640625" style="2"/>
+    <col min="3" max="3" width="48.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1848,7 +2157,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>57</v>
       </c>
@@ -1856,7 +2165,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>59</v>
       </c>
@@ -1864,7 +2173,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>61</v>
       </c>
@@ -1872,7 +2181,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>63</v>
       </c>
@@ -1880,7 +2189,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>65</v>
       </c>
@@ -1888,7 +2197,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>67</v>
       </c>
@@ -1896,7 +2205,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>69</v>
       </c>
@@ -1904,7 +2213,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>71</v>
       </c>
@@ -1912,7 +2221,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>73</v>
       </c>
@@ -1920,7 +2229,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>75</v>
       </c>
@@ -1928,7 +2237,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>77</v>
       </c>
@@ -1936,7 +2245,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>79</v>
       </c>
@@ -1944,7 +2253,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>81</v>
       </c>
@@ -1952,7 +2261,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>83</v>
       </c>
@@ -1965,7 +2274,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F568D1CF-900F-154E-8444-949F6BB9AE2C}">
   <dimension ref="A1:N38"/>
   <sheetViews>
@@ -1973,12 +2282,12 @@
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="16384" width="11" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1994,7 +2303,7 @@
       <c r="M1" s="15"/>
       <c r="N1" s="15"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -2018,7 +2327,7 @@
       <c r="M2" s="17"/>
       <c r="N2" s="17"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="8" t="s">
         <v>16</v>
@@ -2042,7 +2351,7 @@
       <c r="M3" s="17"/>
       <c r="N3" s="17"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="9" t="s">
         <v>26</v>
@@ -2066,7 +2375,7 @@
       <c r="M4" s="17"/>
       <c r="N4" s="17"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="8" t="s">
         <v>8</v>
@@ -2090,7 +2399,7 @@
       <c r="M5" s="17"/>
       <c r="N5" s="17"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="9" t="s">
         <v>24</v>
@@ -2114,7 +2423,7 @@
       <c r="M6" s="17"/>
       <c r="N6" s="17"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="8" t="s">
         <v>2</v>
@@ -2138,7 +2447,7 @@
       <c r="M7" s="17"/>
       <c r="N7" s="17"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="9" t="s">
         <v>87</v>
@@ -2162,7 +2471,7 @@
       <c r="M8" s="17"/>
       <c r="N8" s="17"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="8" t="s">
         <v>4</v>
@@ -2186,7 +2495,7 @@
       <c r="M9" s="17"/>
       <c r="N9" s="17"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="9" t="s">
         <v>10</v>
@@ -2210,7 +2519,7 @@
       <c r="M10" s="17"/>
       <c r="N10" s="17"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="8" t="s">
         <v>28</v>
@@ -2234,7 +2543,7 @@
       <c r="M11" s="17"/>
       <c r="N11" s="17"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="9" t="s">
         <v>14</v>
@@ -2258,7 +2567,7 @@
       <c r="M12" s="17"/>
       <c r="N12" s="17"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="B13" s="8" t="s">
         <v>12</v>
@@ -2282,7 +2591,7 @@
       <c r="M13" s="17"/>
       <c r="N13" s="17"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="9" t="s">
         <v>18</v>
@@ -2306,7 +2615,7 @@
       <c r="M14" s="17"/>
       <c r="N14" s="17"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="8" t="s">
         <v>6</v>
@@ -2330,7 +2639,7 @@
       <c r="M15" s="17"/>
       <c r="N15" s="17"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
       <c r="B16" s="9" t="s">
         <v>22</v>
@@ -2354,7 +2663,7 @@
       <c r="M16" s="17"/>
       <c r="N16" s="17"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
       <c r="B17" s="8" t="s">
         <v>30</v>
@@ -2378,7 +2687,7 @@
       <c r="M17" s="17"/>
       <c r="N17" s="17"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
       <c r="B18" s="9" t="s">
         <v>20</v>
@@ -2402,7 +2711,7 @@
       <c r="M18" s="17"/>
       <c r="N18" s="17"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
       <c r="B19" s="8" t="s">
         <v>32</v>
@@ -2426,7 +2735,7 @@
       <c r="M19" s="17"/>
       <c r="N19" s="17"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="15"/>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
@@ -2441,7 +2750,7 @@
       <c r="M20" s="17"/>
       <c r="N20" s="17"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="15"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -2457,7 +2766,7 @@
       <c r="M21" s="17"/>
       <c r="N21" s="17"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="15"/>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
@@ -2473,7 +2782,7 @@
       <c r="M22" s="17"/>
       <c r="N22" s="17"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="15"/>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
@@ -2489,7 +2798,7 @@
       <c r="M23" s="17"/>
       <c r="N23" s="17"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="15"/>
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
@@ -2505,7 +2814,7 @@
       <c r="M24" s="17"/>
       <c r="N24" s="17"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="15"/>
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
@@ -2521,7 +2830,7 @@
       <c r="M25" s="17"/>
       <c r="N25" s="17"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="15"/>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
@@ -2537,7 +2846,7 @@
       <c r="M26" s="17"/>
       <c r="N26" s="17"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="15"/>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
@@ -2553,7 +2862,7 @@
       <c r="M27" s="17"/>
       <c r="N27" s="17"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="15"/>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
@@ -2569,7 +2878,7 @@
       <c r="M28" s="17"/>
       <c r="N28" s="17"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="15"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
@@ -2585,7 +2894,7 @@
       <c r="M29" s="17"/>
       <c r="N29" s="17"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="15"/>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
@@ -2601,7 +2910,7 @@
       <c r="M30" s="17"/>
       <c r="N30" s="17"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="15"/>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
@@ -2617,7 +2926,7 @@
       <c r="M31" s="17"/>
       <c r="N31" s="17"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="15"/>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
@@ -2633,7 +2942,7 @@
       <c r="M32" s="17"/>
       <c r="N32" s="17"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="15"/>
       <c r="B33" s="17"/>
       <c r="C33" s="17"/>
@@ -2649,7 +2958,7 @@
       <c r="M33" s="17"/>
       <c r="N33" s="17"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="15"/>
       <c r="B34" s="17"/>
       <c r="C34" s="17"/>
@@ -2665,7 +2974,7 @@
       <c r="M34" s="17"/>
       <c r="N34" s="17"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="15"/>
       <c r="B35" s="17"/>
       <c r="C35" s="17"/>
@@ -2681,7 +2990,7 @@
       <c r="M35" s="17"/>
       <c r="N35" s="17"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="15"/>
       <c r="B36" s="17"/>
       <c r="C36" s="17"/>
@@ -2697,7 +3006,7 @@
       <c r="M36" s="17"/>
       <c r="N36" s="17"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="15"/>
       <c r="B37" s="17"/>
       <c r="C37" s="17"/>
@@ -2713,7 +3022,7 @@
       <c r="M37" s="17"/>
       <c r="N37" s="17"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="15"/>
       <c r="B38" s="17"/>
       <c r="C38" s="17"/>

</xml_diff>

<commit_message>
with-Notation for column layout
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0e24e2a113d23d62/Dokumente/GitHub/ESEM-EE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{6919FBE6-99CC-3541-96DE-05FA34DA3742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FED8459-D653-4602-83C2-52E29CF44CF8}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{6919FBE6-99CC-3541-96DE-05FA34DA3742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D35A490-5873-4137-9D13-45AAAD948900}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="9030" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{AA20818D-C879-3C47-BB4F-616D309467DF}"/>
+    <workbookView xWindow="-28920" yWindow="9030" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{AA20818D-C879-3C47-BB4F-616D309467DF}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -468,9 +468,6 @@
     <t xml:space="preserve">Paris Klimaziel - 2 °C </t>
   </si>
   <si>
-    <t>Business as Usual'</t>
-  </si>
-  <si>
     <t>Klimaneutrales Deutschland (2045)</t>
   </si>
   <si>
@@ -478,6 +475,9 @@
   </si>
   <si>
     <t>Flachkollektor</t>
+  </si>
+  <si>
+    <t>"Business as Usual"</t>
   </si>
 </sst>
 </file>
@@ -1337,7 +1337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9E424A2-3675-FF47-8266-60B248167A50}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1465,7 +1465,7 @@
         <v>121</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D5" s="11">
         <v>45</v>
@@ -1495,7 +1495,7 @@
         <v>122</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D6" s="11">
         <v>45</v>
@@ -2110,8 +2110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DB8F52B-EB96-459B-BB6A-A07D4250C420}">
   <dimension ref="B2:M6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2146,7 +2146,7 @@
         <v>127</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D3">
         <v>80</v>
@@ -2179,7 +2179,7 @@
         <v>130</v>
       </c>
       <c r="C6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D6">
         <v>250</v>

</xml_diff>

<commit_message>
Remove heat_pump options from current heat_ttech!
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0e24e2a113d23d62/Dokumente/GitHub/ESEM-EE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{6919FBE6-99CC-3541-96DE-05FA34DA3742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8936144E-CF97-4D36-B532-023D5E3FDD23}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{6919FBE6-99CC-3541-96DE-05FA34DA3742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08E5DAFD-2D30-4573-84CC-98C4B6207051}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="9030" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{AA20818D-C879-3C47-BB4F-616D309467DF}"/>
+    <workbookView xWindow="-28920" yWindow="9030" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{AA20818D-C879-3C47-BB4F-616D309467DF}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="149">
   <si>
     <t>id</t>
   </si>
@@ -1908,8 +1908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CAE16E0-8D9A-B945-AFD0-7E1B2FCCBD6C}">
   <dimension ref="B2:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2060,9 +2060,7 @@
         <v>0.4</v>
       </c>
       <c r="F8"/>
-      <c r="G8" t="s">
-        <v>133</v>
-      </c>
+      <c r="G8"/>
       <c r="H8"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -2077,9 +2075,7 @@
         <v>0.5</v>
       </c>
       <c r="F9"/>
-      <c r="G9" t="s">
-        <v>133</v>
-      </c>
+      <c r="G9"/>
       <c r="H9"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -2094,9 +2090,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="F10"/>
-      <c r="G10" t="s">
-        <v>133</v>
-      </c>
+      <c r="G10"/>
       <c r="H10"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -2620,7 +2614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{949C2119-FDD0-4271-989C-5EFC40CCEDE1}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update - Final PDF and Data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0e24e2a113d23d62/Dokumente/GitHub/ESEM-EE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{6919FBE6-99CC-3541-96DE-05FA34DA3742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08E5DAFD-2D30-4573-84CC-98C4B6207051}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{6919FBE6-99CC-3541-96DE-05FA34DA3742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D84B945-76CE-4E9B-B6E3-15F7EEB83375}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="9030" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{AA20818D-C879-3C47-BB4F-616D309467DF}"/>
+    <workbookView xWindow="5895" yWindow="2415" windowWidth="27900" windowHeight="12420" activeTab="1" xr2:uid="{AA20818D-C879-3C47-BB4F-616D309467DF}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -1909,7 +1909,7 @@
   <dimension ref="B2:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1951,11 +1951,11 @@
         <v>107</v>
       </c>
       <c r="D3">
-        <v>30</v>
+        <v>24.29</v>
       </c>
       <c r="E3"/>
       <c r="F3">
-        <v>32.54</v>
+        <v>41.19</v>
       </c>
       <c r="G3" t="s">
         <v>132</v>
@@ -1972,11 +1972,11 @@
         <v>106</v>
       </c>
       <c r="D4">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="E4"/>
       <c r="F4">
-        <v>32.630000000000003</v>
+        <v>36.19</v>
       </c>
       <c r="G4" t="s">
         <v>132</v>
@@ -1993,11 +1993,11 @@
         <v>105</v>
       </c>
       <c r="D5">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E5"/>
       <c r="F5">
-        <v>5</v>
+        <v>7.07</v>
       </c>
       <c r="G5" t="s">
         <v>132</v>
@@ -2013,12 +2013,10 @@
       <c r="C6" t="s">
         <v>104</v>
       </c>
-      <c r="D6">
-        <v>10</v>
-      </c>
+      <c r="D6"/>
       <c r="E6"/>
       <c r="F6">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s">
         <v>132</v>
@@ -2039,7 +2037,7 @@
       </c>
       <c r="E7"/>
       <c r="F7">
-        <v>9.5</v>
+        <v>7.45</v>
       </c>
       <c r="G7" t="s">
         <v>133</v>
@@ -2101,11 +2099,11 @@
         <v>100</v>
       </c>
       <c r="D11">
-        <v>198</v>
+        <v>344.7</v>
       </c>
       <c r="E11"/>
       <c r="F11">
-        <v>9.1999999999999993</v>
+        <v>8</v>
       </c>
       <c r="G11" t="s">
         <v>133</v>
@@ -2114,6 +2112,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2940,7 +2939,7 @@
   <dimension ref="B2:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2978,7 +2977,7 @@
         <v>143</v>
       </c>
       <c r="D3">
-        <v>80</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
@@ -2989,7 +2988,7 @@
         <v>138</v>
       </c>
       <c r="D4">
-        <v>400</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
@@ -3000,7 +2999,7 @@
         <v>139</v>
       </c>
       <c r="D5">
-        <v>300</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
@@ -3011,7 +3010,7 @@
         <v>140</v>
       </c>
       <c r="D6">
-        <v>250</v>
+        <v>505.13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>